<commit_message>
Add test scripts for insurance fund restrictions, text normalization, and EPM consolidator
- Implemented `test_fondos_aseguradoras.py` to validate insurance restrictions per fund.
- Created `test_normalization.py` for text normalization functionality and search tests.
- Developed `test_quick_epm.py` for quick testing of EPM consolidator with example data.
</commit_message>
<xml_diff>
--- a/Bases Consolidados/PANTILLA EPM N.xlsx
+++ b/Bases Consolidados/PANTILLA EPM N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\MCP\Bases Consolidados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17D3EC9-CAE4-41F2-8FC9-24E106019178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5875C4B6-9279-43F4-8EB8-B990172E7029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25690" yWindow="0" windowWidth="18740" windowHeight="15370" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Autos" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Fecha De Cotización</t>
   </si>
@@ -98,9 +98,6 @@
     <t>DEDUCIBLES</t>
   </si>
   <si>
-    <t>Forma de pago</t>
-  </si>
-  <si>
     <t>Importante</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Bolivar</t>
   </si>
   <si>
-    <t>Solidaria</t>
-  </si>
-  <si>
     <t>VALOR A PAGAR  (IVA INCLUIDO)</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>Autos Global</t>
   </si>
   <si>
-    <t>Autos Clasico</t>
-  </si>
-  <si>
     <t>Autos Esencial + Total</t>
   </si>
   <si>
@@ -144,13 +135,19 @@
   </si>
   <si>
     <t>Autos llave en mano</t>
+  </si>
+  <si>
+    <t>CONDICIONES ECONOMICAS</t>
+  </si>
+  <si>
+    <t>Autos Parcial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +204,14 @@
       <name val="Arial Rounded MT Bold"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial Rounded MT Bold"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +254,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -351,13 +366,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,12 +380,40 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -387,47 +427,31 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,22 +530,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>493058</xdr:colOff>
+      <xdr:colOff>89648</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>112061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>128884</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1176619</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>655547</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C56078E4-EE87-059A-2467-72B7895E1998}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD3A7CB0-1B01-7820-0194-F0A7E857B784}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -543,8 +567,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10070352" y="1"/>
-          <a:ext cx="2006227" cy="865296"/>
+          <a:off x="9681883" y="112061"/>
+          <a:ext cx="1086971" cy="543486"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,549 +884,550 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971C112-9AF6-42D6-81AB-E2C154B579CA}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="C6" sqref="C6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="18.5703125" customWidth="1"/>
+    <col min="2" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="1" spans="1:8" ht="59.1" customHeight="1">
+      <c r="A1" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="20"/>
+      <c r="B20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="7"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="7"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="7"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="7"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75">
+      <c r="A29" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="7"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75">
+      <c r="A32" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="B33" s="15">
+        <v>45913</v>
+      </c>
+      <c r="C33" s="15">
+        <v>45913</v>
+      </c>
+      <c r="D33" s="15">
+        <v>45913</v>
+      </c>
+      <c r="E33" s="15">
+        <v>45913</v>
+      </c>
+      <c r="F33" s="15">
+        <v>45913</v>
+      </c>
+      <c r="G33" s="15">
+        <v>45913</v>
+      </c>
+      <c r="H33" s="15">
+        <v>45913</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="B34" s="15">
+        <v>45974</v>
+      </c>
+      <c r="C34" s="15">
+        <v>45971</v>
+      </c>
+      <c r="D34" s="15">
+        <v>45974</v>
+      </c>
+      <c r="E34" s="15">
+        <v>45974</v>
+      </c>
+      <c r="F34" s="15">
+        <v>45974</v>
+      </c>
+      <c r="G34" s="15">
+        <v>45974</v>
+      </c>
+      <c r="H34" s="15">
+        <v>45974</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="B35" s="17">
+        <v>61</v>
+      </c>
+      <c r="C35" s="17">
+        <v>58</v>
+      </c>
+      <c r="D35" s="17">
+        <v>61</v>
+      </c>
+      <c r="E35" s="17">
+        <v>61</v>
+      </c>
+      <c r="F35" s="17">
+        <v>61</v>
+      </c>
+      <c r="G35" s="17">
+        <v>61</v>
+      </c>
+      <c r="H35" s="17">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-    </row>
-    <row r="41" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+    </row>
+    <row r="40" spans="1:8" ht="44.25" customHeight="1">
+      <c r="A40" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1411,9 +1436,8 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1422,9 +1446,8 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1433,9 +1456,8 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1444,9 +1466,8 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1455,9 +1476,8 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1466,9 +1486,8 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1477,9 +1496,8 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1488,22 +1506,10 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="A1:I1"/>
+  <mergeCells count="35">
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A16:B16"/>
@@ -1512,39 +1518,32 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="A32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1553,6 +1552,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A46240E9C16ACF4580208BCDD1584C19" ma:contentTypeVersion="1" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c123b30116eb1696ed6760edbcdae06c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cb24288e-bf72-47ae-a461-19b0293297a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9259aa4610e07bbb8461321e94cbc80" ns3:_="">
     <xsd:import namespace="cb24288e-bf72-47ae-a461-19b0293297a2"/>
@@ -1678,7 +1683,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1687,13 +1692,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="cb24288e-bf72-47ae-a461-19b0293297a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F720539-AD5F-4FC3-9414-E2EE1548D97C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1711,26 +1726,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="cb24288e-bf72-47ae-a461-19b0293297a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Implementar nueva nomenclatura para planes de Sura y mejorar manejo de valores asegurados
- Actualizar nomenclatura de planes de Sura a "Global Franquicia", "Autos Global" y "Autos Clásico".
- Modificar procesos de extracción y consolidación para reflejar la nueva nomenclatura.
- Añadir verificación y solicitud de valor asegurado al usuario si no está disponible.
- Mejorar manejo de modales y tiempos de espera en la automatización de Sura.
- Implementar pruebas para validar la nueva nomenclatura y mapeos en el template handler.
</commit_message>
<xml_diff>
--- a/Bases Consolidados/PANTILLA EPM N.xlsx
+++ b/Bases Consolidados/PANTILLA EPM N.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\Bases Consolidados Nuevas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\MCP\Bases Consolidados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AFF91C-2236-40A8-8608-71B566FA6CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F539A5-6802-4B66-B367-F6474365D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
+    <workbookView xWindow="-12890" yWindow="120" windowWidth="12980" windowHeight="15370" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Autos" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t>Fecha De Cotización</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>VALOR ASEGURADO AUTO</t>
+  </si>
+  <si>
+    <t>Autos Clasico</t>
   </si>
 </sst>
 </file>
@@ -613,52 +616,52 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +686,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1447800</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -742,7 +745,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1447800</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1095,214 +1098,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971C112-9AF6-42D6-81AB-E2C154B579CA}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="3" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="59.1" customHeight="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:8" ht="59.1" customHeight="1">
+      <c r="A1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="31" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="33" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="31" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="33" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="31" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="B6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="31" t="s">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="33" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="31" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="33" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="31" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="B12" s="38"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="31" t="s">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="33" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="31" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="33" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="B17" s="44"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="37" t="s">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1312,38 +1333,44 @@
         <v>22</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="37"/>
+    <row r="20" spans="1:8">
+      <c r="A20" s="36"/>
       <c r="B20" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="F20" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="G20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="1:7" ht="45">
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="1:8" ht="45">
       <c r="A21" s="17" t="s">
         <v>50</v>
       </c>
@@ -1353,9 +1380,7 @@
       <c r="C21" s="18">
         <v>3040000000</v>
       </c>
-      <c r="D21" s="18">
-        <v>5000000000</v>
-      </c>
+      <c r="D21" s="18"/>
       <c r="E21" s="18">
         <v>5000000000</v>
       </c>
@@ -1363,10 +1388,13 @@
         <v>5000000000</v>
       </c>
       <c r="G21" s="18">
+        <v>5000000000</v>
+      </c>
+      <c r="H21" s="18">
         <v>4000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="17" t="s">
         <v>33</v>
       </c>
@@ -1376,9 +1404,7 @@
       <c r="C22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>51</v>
-      </c>
+      <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
         <v>51</v>
       </c>
@@ -1388,8 +1414,11 @@
       <c r="G22" s="18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="22.5">
       <c r="A23" s="15" t="s">
         <v>34</v>
       </c>
@@ -1399,9 +1428,7 @@
       <c r="C23" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="D23" s="16"/>
       <c r="E23" s="18" t="s">
         <v>77</v>
       </c>
@@ -1411,8 +1438,11 @@
       <c r="G23" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="22.5">
       <c r="A24" s="15" t="s">
         <v>35</v>
       </c>
@@ -1423,22 +1453,23 @@
         <f t="shared" ref="C24:C27" si="0">+C23</f>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="E24" s="18" t="str">
-        <f>E23</f>
-        <v>VALOR ASEGURADO AUTO</v>
       </c>
       <c r="F24" s="18" t="str">
         <f>F23</f>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="18" t="str">
+        <f>G23</f>
+        <v>VALOR ASEGURADO AUTO</v>
+      </c>
+      <c r="H24" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8" ht="22.5">
       <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
@@ -1449,23 +1480,24 @@
         <f t="shared" si="0"/>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="D25" s="18" t="str">
-        <f>D23</f>
+      <c r="D25" s="16"/>
+      <c r="E25" s="18" t="str">
+        <f>E23</f>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="E25" s="18" t="str">
-        <f t="shared" ref="E25:E27" si="1">+E24</f>
+      <c r="F25" s="18" t="str">
+        <f t="shared" ref="F25:F27" si="1">+F24</f>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="F25" s="18" t="str">
-        <f t="shared" ref="F25:F27" si="2">+F24</f>
+      <c r="G25" s="18" t="str">
+        <f t="shared" ref="G25:G27" si="2">+G24</f>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="H25" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8" ht="22.5">
       <c r="A26" s="15" t="s">
         <v>35</v>
       </c>
@@ -1476,22 +1508,23 @@
         <f t="shared" si="0"/>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="18" t="str">
+      <c r="F26" s="18" t="str">
         <f t="shared" si="1"/>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="F26" s="18" t="str">
+      <c r="G26" s="18" t="str">
         <f t="shared" si="2"/>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="H26" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8" ht="22.5">
       <c r="A27" s="15" t="s">
         <v>37</v>
       </c>
@@ -1502,23 +1535,24 @@
         <f t="shared" si="0"/>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="D27" s="18" t="str">
-        <f>D25</f>
+      <c r="D27" s="16"/>
+      <c r="E27" s="18" t="str">
+        <f>E25</f>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="E27" s="18" t="str">
+      <c r="F27" s="18" t="str">
         <f t="shared" si="1"/>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="F27" s="18" t="str">
+      <c r="G27" s="18" t="str">
         <f t="shared" si="2"/>
         <v>VALOR ASEGURADO AUTO</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="H27" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
@@ -1528,9 +1562,7 @@
       <c r="C28" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>52</v>
-      </c>
+      <c r="D28" s="16"/>
       <c r="E28" s="18" t="s">
         <v>52</v>
       </c>
@@ -1538,10 +1570,13 @@
         <v>52</v>
       </c>
       <c r="G28" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="22.5">
+    <row r="29" spans="1:8" ht="22.5">
       <c r="A29" s="15" t="s">
         <v>39</v>
       </c>
@@ -1551,20 +1586,21 @@
       <c r="C29" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="18">
-        <v>1200000</v>
-      </c>
+      <c r="D29" s="16"/>
       <c r="E29" s="18">
         <v>1200000</v>
       </c>
       <c r="F29" s="18">
         <v>1200000</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="G29" s="18">
+        <v>1200000</v>
+      </c>
+      <c r="H29" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="15" t="s">
         <v>40</v>
       </c>
@@ -1574,9 +1610,7 @@
       <c r="C30" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>54</v>
-      </c>
+      <c r="D30" s="16"/>
       <c r="E30" s="18" t="s">
         <v>54</v>
       </c>
@@ -1584,10 +1618,13 @@
         <v>54</v>
       </c>
       <c r="G30" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" s="15" t="s">
         <v>41</v>
       </c>
@@ -1597,9 +1634,7 @@
       <c r="C31" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>60</v>
-      </c>
+      <c r="D31" s="16"/>
       <c r="E31" s="18" t="s">
         <v>60</v>
       </c>
@@ -1607,10 +1642,13 @@
         <v>60</v>
       </c>
       <c r="G31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" s="15" t="s">
         <v>42</v>
       </c>
@@ -1620,9 +1658,7 @@
       <c r="C32" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="18" t="s">
-        <v>51</v>
-      </c>
+      <c r="D32" s="16"/>
       <c r="E32" s="18" t="s">
         <v>51</v>
       </c>
@@ -1632,8 +1668,11 @@
       <c r="G32" s="18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="15" t="s">
         <v>43</v>
       </c>
@@ -1643,20 +1682,21 @@
       <c r="C33" s="16">
         <v>50000000</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="18">
-        <v>50000000</v>
+      <c r="D33" s="16"/>
+      <c r="E33" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="F33" s="18">
         <v>50000000</v>
       </c>
-      <c r="G33" s="38" t="s">
+      <c r="G33" s="18">
+        <v>50000000</v>
+      </c>
+      <c r="H33" s="30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" s="15" t="s">
         <v>44</v>
       </c>
@@ -1666,18 +1706,19 @@
       <c r="C34" s="16">
         <v>35000000</v>
       </c>
-      <c r="D34" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="D34" s="16"/>
       <c r="E34" s="18" t="s">
         <v>55</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="38"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="G34" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="15" t="s">
         <v>45</v>
       </c>
@@ -1687,9 +1728,7 @@
       <c r="C35" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="D35" s="16"/>
       <c r="E35" s="18" t="s">
         <v>55</v>
       </c>
@@ -1699,8 +1738,11 @@
       <c r="G35" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="15" t="s">
         <v>46</v>
       </c>
@@ -1710,9 +1752,7 @@
       <c r="C36" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="D36" s="16"/>
       <c r="E36" s="18" t="s">
         <v>55</v>
       </c>
@@ -1722,8 +1762,11 @@
       <c r="G36" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="17" t="s">
         <v>47</v>
       </c>
@@ -1733,9 +1776,7 @@
       <c r="C37" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="D37" s="18"/>
       <c r="E37" s="18" t="s">
         <v>55</v>
       </c>
@@ -1745,8 +1786,11 @@
       <c r="G37" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="17" t="s">
         <v>48</v>
       </c>
@@ -1756,9 +1800,7 @@
       <c r="C38" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="D38" s="18"/>
       <c r="E38" s="18" t="s">
         <v>55</v>
       </c>
@@ -1768,8 +1810,11 @@
       <c r="G38" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="17" t="s">
         <v>49</v>
       </c>
@@ -1779,20 +1824,21 @@
       <c r="C39" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="D39" s="18"/>
       <c r="E39" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>52</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>52</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1800,19 +1846,21 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="39" t="s">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="24" t="s">
         <v>62</v>
       </c>
@@ -1822,9 +1870,7 @@
       <c r="C42" s="22">
         <v>0</v>
       </c>
-      <c r="D42" s="22">
-        <v>0</v>
-      </c>
+      <c r="D42" s="22"/>
       <c r="E42" s="22">
         <v>0</v>
       </c>
@@ -1834,8 +1880,11 @@
       <c r="G42" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="24" t="s">
         <v>63</v>
       </c>
@@ -1845,9 +1894,7 @@
       <c r="C43" s="22">
         <v>0</v>
       </c>
-      <c r="D43" s="22">
-        <v>0</v>
-      </c>
+      <c r="D43" s="22"/>
       <c r="E43" s="22">
         <v>0</v>
       </c>
@@ -1857,8 +1904,11 @@
       <c r="G43" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="45">
+      <c r="H43" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="45">
       <c r="A44" s="24" t="s">
         <v>64</v>
       </c>
@@ -1868,20 +1918,21 @@
       <c r="C44" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>66</v>
+      <c r="D44" s="23"/>
+      <c r="E44" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="F44" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="23">
+      <c r="G44" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="H44" s="23">
         <v>800000</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1889,19 +1940,21 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75">
-      <c r="A46" s="40" t="s">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75">
+      <c r="A46" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="24" t="s">
         <v>68</v>
       </c>
@@ -1911,20 +1964,21 @@
       <c r="C47" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="26" t="s">
-        <v>55</v>
-      </c>
+      <c r="D47" s="26"/>
       <c r="E47" s="26" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="F47" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="G47" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="G47" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="24" t="s">
         <v>70</v>
       </c>
@@ -1934,20 +1988,21 @@
       <c r="C48" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="26" t="s">
-        <v>55</v>
-      </c>
+      <c r="D48" s="26"/>
       <c r="E48" s="26" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F48" s="26" t="s">
         <v>71</v>
       </c>
       <c r="G48" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H48" s="26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" s="24" t="s">
         <v>72</v>
       </c>
@@ -1957,9 +2012,7 @@
       <c r="C49" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="26" t="s">
-        <v>74</v>
-      </c>
+      <c r="D49" s="26"/>
       <c r="E49" s="26" t="s">
         <v>74</v>
       </c>
@@ -1967,10 +2020,13 @@
         <v>74</v>
       </c>
       <c r="G49" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" s="27" t="s">
         <v>73</v>
       </c>
@@ -1980,20 +2036,21 @@
       <c r="C50" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="D50" s="26"/>
       <c r="E50" s="26" t="s">
         <v>52</v>
       </c>
       <c r="F50" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="G50" s="28" t="s">
+      <c r="G50" s="26" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2001,19 +2058,21 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75">
-      <c r="A52" s="43" t="s">
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="15.75">
+      <c r="A52" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="6" t="s">
         <v>13</v>
       </c>
@@ -2023,8 +2082,9 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="6" t="s">
         <v>14</v>
       </c>
@@ -2044,10 +2104,13 @@
         <v>46266</v>
       </c>
       <c r="G54" s="10">
+        <v>46266</v>
+      </c>
+      <c r="H54" s="10">
         <v>46296</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" s="6" t="s">
         <v>15</v>
       </c>
@@ -2057,8 +2120,9 @@
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="12"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="14" t="s">
         <v>25</v>
       </c>
@@ -2068,8 +2132,9 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" s="13"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="14" t="s">
         <v>16</v>
       </c>
@@ -2079,39 +2144,43 @@
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="11"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="1"/>
+      <c r="F58" s="2"/>
       <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="42" t="s">
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="42"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
-    </row>
-    <row r="60" spans="1:7" ht="44.25" customHeight="1">
-      <c r="A60" s="41" t="s">
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+    </row>
+    <row r="60" spans="1:8" ht="44.25" customHeight="1">
+      <c r="A60" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="41"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="B60" s="33"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2119,8 +2188,9 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2128,8 +2198,9 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2137,8 +2208,9 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2146,8 +2218,9 @@
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2155,8 +2228,9 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2164,8 +2238,9 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2173,8 +2248,9 @@
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2182,8 +2258,9 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2191,30 +2268,11 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A16:B16"/>
@@ -2223,13 +2281,33 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A52:H52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2244,15 +2322,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A46240E9C16ACF4580208BCDD1584C19" ma:contentTypeVersion="1" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c123b30116eb1696ed6760edbcdae06c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cb24288e-bf72-47ae-a461-19b0293297a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9259aa4610e07bbb8461321e94cbc80" ns3:_="">
     <xsd:import namespace="cb24288e-bf72-47ae-a461-19b0293297a2"/>
@@ -2378,6 +2447,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
   <ds:schemaRefs>
@@ -2395,14 +2473,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F720539-AD5F-4FC3-9414-E2EE1548D97C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2418,4 +2488,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>